<commit_message>
agregando proyecto analisis vehiculos rojos
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\UVG-CC3074-PY01-Analisis-Exploratorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\UVG-CC3074-PY01-Analisis-Exploratorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{051FA633-BD60-47BE-8D94-9B274211A4E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9218AE68-E03D-4593-B09B-44B5DD4B87BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{77A07049-394D-414A-9A68-90D827156F73}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="transito" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>